<commit_message>
revert back to 1.4
</commit_message>
<xml_diff>
--- a/static/crestfallen_sandbox.xlsx
+++ b/static/crestfallen_sandbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheri\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1F2B32-CD16-457A-8D6A-DF406161C63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90594B4-1036-440A-9E7C-EE393CA0E77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9BC04F54-DC90-40C8-A3AA-75E10889ECBB}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="347">
   <si>
     <t>Player Name:</t>
   </si>
@@ -1277,12 +1277,6 @@
   </si>
   <si>
     <t>→</t>
-  </si>
-  <si>
-    <t>Crestfallen.larp.logistics@gmail.com</t>
-  </si>
-  <si>
-    <t>CrestfallenLarp@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1931,7 +1925,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2203,14 +2197,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2218,6 +2209,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2242,16 +2240,16 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="1"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="5"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -2272,13 +2270,6 @@
         <b/>
         <i val="0"/>
         <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="5"/>
       </font>
     </dxf>
     <dxf>
@@ -2354,57 +2345,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>131384</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7A74072-8329-B7F4-8FE2-54B345B529B6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:alphaModFix amt="5000"/>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="904875"/>
-          <a:ext cx="20478750" cy="19038509"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -2599,16 +2539,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>230700</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>706950</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>933450</xdr:colOff>
-      <xdr:row>130</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1600200</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2624,7 +2564,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2638,8 +2578,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="373575" y="21983700"/>
-          <a:ext cx="4084125" cy="3981449"/>
+          <a:off x="2440500" y="12896850"/>
+          <a:ext cx="4074600" cy="3981449"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2892,20 +2832,6 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>→</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="en-US" sz="1100" b="1">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
@@ -2927,33 +2853,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> or Kinfolk Lineages, choose your lineage bonus by clicking on either "Adaptable' for humans or "Variable" for kinfolk in the dropdown list that appears </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>→</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>above the skills table. If you change lineages,, make sure you change the skill back to Adaptable or Variable respectively.</a:t>
+            <a:t> or Kinfolk Lineages, choose your lineage bonus by clicking on either "Adaptable' for humans or "Variable" for kinfolk in the dropdown list that appears above the skills table. If you change lineages,, make sure you change the skill back to Adaptable or Variable respectively.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:solidFill>
@@ -3294,56 +3194,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>833438</xdr:colOff>
-      <xdr:row>117</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>116804</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>109017</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D91637F2-E32E-94A4-9B79-E3C78CB8D7E3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4357688" y="23550563"/>
-          <a:ext cx="4712616" cy="585267"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3649,8 +3499,8 @@
   </sheetPr>
   <dimension ref="A5:AB144"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="69" zoomScaleNormal="69" zoomScalePageLayoutView="59" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="59" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3735,7 +3585,7 @@
         <v>3</v>
       </c>
       <c r="I7" s="61">
-        <f>F15+J13+A7</f>
+        <f>F15+J13+A7-H58</f>
         <v>0</v>
       </c>
       <c r="J7" s="14"/>
@@ -3796,13 +3646,13 @@
         <v>5</v>
       </c>
       <c r="J9" s="15"/>
-      <c r="L9" s="99" t="s">
+      <c r="L9" s="98" t="s">
         <v>326</v>
       </c>
-      <c r="M9" s="99"/>
-      <c r="N9" s="99"/>
-      <c r="O9" s="99"/>
-      <c r="P9" s="99"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="98"/>
+      <c r="O9" s="98"/>
+      <c r="P9" s="98"/>
       <c r="Q9"/>
       <c r="R9"/>
       <c r="S9" s="41" t="s">
@@ -5610,7 +5460,7 @@
       <c r="E58" s="12"/>
       <c r="F58" s="17"/>
       <c r="G58" s="12"/>
-      <c r="H58" s="98">
+      <c r="H58" s="99">
         <f>SUM(H13:H57)</f>
         <v>0</v>
       </c>
@@ -6185,109 +6035,97 @@
       </c>
       <c r="T112" s="87"/>
     </row>
-    <row r="113" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S113" s="88" t="s">
         <v>314</v>
       </c>
       <c r="T113" s="87"/>
     </row>
-    <row r="114" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S114" s="88" t="s">
         <v>315</v>
       </c>
       <c r="T114" s="87"/>
     </row>
-    <row r="115" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S115" s="88" t="s">
         <v>84</v>
       </c>
       <c r="T115" s="87"/>
     </row>
-    <row r="116" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S116" s="88" t="s">
         <v>106</v>
       </c>
       <c r="T116" s="87"/>
     </row>
-    <row r="117" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S117" s="88" t="s">
         <v>184</v>
       </c>
       <c r="T117" s="87"/>
     </row>
-    <row r="118" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S118" s="88" t="s">
         <v>44</v>
       </c>
       <c r="T118" s="87"/>
     </row>
-    <row r="119" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S119" s="88" t="s">
         <v>128</v>
       </c>
       <c r="T119" s="87"/>
     </row>
-    <row r="120" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S120" s="88" t="s">
         <v>316</v>
       </c>
       <c r="T120" s="87"/>
     </row>
-    <row r="121" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S121" s="88" t="s">
         <v>317</v>
       </c>
       <c r="T121" s="87"/>
     </row>
-    <row r="122" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F122" s="100" t="s">
-        <v>348</v>
-      </c>
-      <c r="G122" s="100"/>
-      <c r="H122" s="100"/>
-      <c r="I122" s="100"/>
+    <row r="122" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S122" s="88" t="s">
         <v>318</v>
       </c>
       <c r="T122" s="87"/>
     </row>
-    <row r="123" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F123" s="100" t="s">
-        <v>347</v>
-      </c>
-      <c r="G123" s="100"/>
-      <c r="H123" s="100"/>
-      <c r="I123" s="100"/>
+    <row r="123" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S123" s="88" t="s">
         <v>118</v>
       </c>
       <c r="T123" s="87"/>
     </row>
-    <row r="124" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S124" s="88" t="s">
         <v>319</v>
       </c>
       <c r="T124" s="87"/>
     </row>
-    <row r="125" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="125" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S125" s="88" t="s">
         <v>320</v>
       </c>
       <c r="T125" s="87"/>
     </row>
-    <row r="126" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="126" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S126" s="88" t="s">
         <v>224</v>
       </c>
       <c r="T126" s="87"/>
     </row>
-    <row r="127" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="127" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S127" s="88" t="s">
         <v>321</v>
       </c>
       <c r="T127" s="87"/>
     </row>
-    <row r="128" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="19:20" x14ac:dyDescent="0.25">
       <c r="S128" s="88" t="s">
         <v>322</v>
       </c>
@@ -6373,7 +6211,7 @@
       <c r="S144" s="40"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="aJXrtNH4Gy68oKYWF5Lqhek4Lu8sbmlVVAG55xjC4ryoD6PYrQCmIM9FY5khi+VacD3hJqFdKM64FGk5gKl9tA==" saltValue="OFA3da48XI1KHWAuotnQHA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="1AlsmHm5/lWmjV69nuJy6v9vZ+pCn7QEgjbcGC3rKPDS0rOrEi3EzAKTD/VlZ/kOLpB6VN4doGVJr61tvtwAow==" saltValue="TxHBsYwJ9E1aA3xQ8X5EUg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="I13:I57" name="Multiples2"/>
     <protectedRange sqref="F13:F57" name="Multiples1"/>
@@ -6383,10 +6221,8 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AA7:AA21">
     <sortCondition ref="AA7:AA21"/>
   </sortState>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="L9:P9"/>
-    <mergeCell ref="F123:I123"/>
-    <mergeCell ref="F122:I122"/>
   </mergeCells>
   <conditionalFormatting sqref="C17:F17">
     <cfRule type="expression" dxfId="13" priority="24">
@@ -6412,19 +6248,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="8" priority="13">
+      <formula>$D$10="Adaptable"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>$D$10&lt;&gt;"Adaptable"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="13">
-      <formula>$D$10="Adaptable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="6" priority="10">
+      <formula>$D$11="Variable"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>$D$11&lt;&gt;"Variable"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="10">
-      <formula>$D$11="Variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C11">
@@ -6433,11 +6269,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:I11">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>$G$10=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$G$10=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$G$10=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:I11">
@@ -6599,15 +6435,13 @@
     <hyperlink ref="T22" r:id="rId141" location="sleepremove-sleep" display="https://crestfallenlarp.com/rules/spells/ - sleepremove-sleep" xr:uid="{57C50D66-D311-4720-9312-56BCCB95CC6D}"/>
     <hyperlink ref="T23" r:id="rId142" location="slowremove-slow" display="https://crestfallenlarp.com/rules/spells/ - slowremove-slow" xr:uid="{0BDB467F-ACA3-4DB9-8E5B-19C8C5F60743}"/>
     <hyperlink ref="T24" r:id="rId143" location="weaknessremove-weakness" display="https://crestfallenlarp.com/rules/spells/ - weaknessremove-weakness" xr:uid="{4C01C8BA-CA36-4EA8-B701-2CDE75A81698}"/>
-    <hyperlink ref="F123" r:id="rId144" xr:uid="{62CE31E8-C339-44F3-9ADE-4B252A3951F1}"/>
-    <hyperlink ref="F122" r:id="rId145" xr:uid="{3D3CE19B-B5CE-4F34-8124-69CA81AC0773}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="69" orientation="portrait" verticalDpi="300" r:id="rId146"/>
+  <pageSetup scale="69" orientation="portrait" verticalDpi="300" r:id="rId144"/>
   <ignoredErrors>
     <ignoredError sqref="E16" formula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId147"/>
+  <drawing r:id="rId145"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">

</xml_diff>